<commit_message>
Included FRBEDO08 + corresponding code and data revision
</commit_message>
<xml_diff>
--- a/data/fill_nowcast.xlsx
+++ b/data/fill_nowcast.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA0FE70-508A-4EDC-9327-E64E6EB75CCA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4047C6E2-421D-4E0F-B726-EF68D6445C7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="26310" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>alfred</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>CPI</t>
+  </si>
+  <si>
+    <t>PRFIC1</t>
+  </si>
+  <si>
+    <t>PNFIC1</t>
+  </si>
+  <si>
+    <t>RNRESIN</t>
+  </si>
+  <si>
+    <t>RRESINV</t>
   </si>
 </sst>
 </file>
@@ -384,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +462,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>